<commit_message>
Fix import/export column names. Remove bp activity comment secretariat
</commit_message>
<xml_diff>
--- a/core/api/tests/files/Test_BP2025-2027_invalid_template.xlsx
+++ b/core/api/tests/files/Test_BP2025-2027_invalid_template.xlsx
@@ -69,52 +69,52 @@
     <t xml:space="preserve">Required by Model</t>
   </si>
   <si>
-    <t xml:space="preserve">Value ($000) 2024 Adjusted</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ODP 2025 Adjusted</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MT for HFC 2025 Adjusted</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CO₂-eq 2025 Adjusted</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Value ($000) 2026 Adjusted</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ODP 2026 Adjusted</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MT for HFC 2026 Adjusted</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CO₂-eq 2026 Adjusted</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Value ($000) 2027 Adjusted</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ODP 2027 Adjusted</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MT for HFC 2027 Adjusted</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CO₂-eq 2027 Adjusted</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Value ($000) After 2027 Adjusted</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ODP After 2027 Adjusted</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MT for HFC After 2027 Adjusted</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CO₂-eq After 2027 Adjusted</t>
+    <t xml:space="preserve">Value ($000) 2024 adjusted</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ODP 2025 adjusted</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MT for HFC 2025 adjusted</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CO2-EQ 2025 adjusted</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Value ($000) 2026 adjusted</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ODP 2026 adjusted</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MT for HFC 2026 adjusted</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CO₂-eq 2026 adjusted</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Value ($000) 2027 adjusted</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ODP 2027 adjusted</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MT for HFC 2027 adjusted</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CO2-EQ 2027 adjusted</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Value ($000) after 2027 adjusted</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ODP after 2027 adjusted</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MT for HFC after 2027 adjusted</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CO2-EQ after 2027 adjusted</t>
   </si>
   <si>
     <t xml:space="preserve">Project Status (A/P)</t>
@@ -2000,6 +2000,7 @@
       <color rgb="FF000000"/>
       <name val="Calibri-Bold"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -2430,8 +2431,8 @@
   </sheetPr>
   <dimension ref="A1:AH652"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="X1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AC6" activeCellId="0" sqref="AC6"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AA1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="W4" activeCellId="0" sqref="W4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.859375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>